<commit_message>
Refactored WorkBook for better mapping of table/column values
</commit_message>
<xml_diff>
--- a/src/test/resources/workbook.xlsx
+++ b/src/test/resources/workbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo/Workspace/plenix/la-holandesa/sap-orders/sap-orders/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo/Workspace/plenix/la-holandesa/excel-extractor/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8457A460-9480-E744-B6B7-54C938283BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D06BE4F-B505-E448-8F64-60D6F9A7F333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{30B031B8-246C-9D4A-BDDF-9204ABC8E826}"/>
   </bookViews>
@@ -87,9 +87,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="172" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -143,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -160,6 +161,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +479,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,6 +487,7 @@
     <col min="1" max="1" width="10.83203125" style="7"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -591,9 +594,8 @@
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="F8" s="9">
-        <f>F7+1</f>
-        <v>44567</v>
+      <c r="F8" s="10">
+        <v>44567.416666666664</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>